<commit_message>
Bug Fixes. And now we can use foreach! Awesome!!
</commit_message>
<xml_diff>
--- a/test/Test/Files/SampleData.xlsx
+++ b/test/Test/Files/SampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdal\OneDrive\Documents\ContexturesSampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayrto\source\repos\NpoiMadeSimple\test\Test\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E70720A-763A-460D-9657-3B9DD8EFFB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F2BFF4-F167-4F82-8341-A9F2A2C180CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24030" yWindow="-3540" windowWidth="22845" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="74">
   <si>
     <t>Region</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>More Excel Sample Files</t>
+  </si>
+  <si>
+    <t>Less than 10 units</t>
   </si>
 </sst>
 </file>
@@ -259,8 +262,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -372,7 +375,7 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -423,7 +426,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -433,10 +436,10 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -473,14 +476,35 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Ctx_Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{EB666C6D-407C-40C7-A692-53700D36DD5D}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 4" xfId="4" xr:uid="{1A867160-CFF8-4CFB-9486-A3FC92514B8F}"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -637,9 +661,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G44" totalsRowShown="0">
-  <autoFilter ref="A1:G44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H44" totalsRowShown="0">
+  <autoFilter ref="A1:H44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="OrderDate"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Region"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Rep"/>
@@ -647,13 +671,16 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Units"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Total"/>
+    <tableColumn id="8" xr3:uid="{7F11AC43-12E5-4B3E-8974-E2A5666C58E1}" name="Less than 10 units" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Units]]&lt;10</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -976,7 +1003,7 @@
   <sheetPr codeName="Sheet30"/>
   <dimension ref="B1:C27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -1113,11 +1140,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,10 +1156,11 @@
     <col min="5" max="5" width="7.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="9" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="8" max="8" width="18.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
@@ -1154,8 +1182,11 @@
       <c r="G1" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>43471</v>
       </c>
@@ -1177,8 +1208,12 @@
       <c r="G2" s="19">
         <v>189.05</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>43488</v>
       </c>
@@ -1200,8 +1235,12 @@
       <c r="G3" s="19">
         <v>999.49999999999989</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>43505</v>
       </c>
@@ -1223,8 +1262,12 @@
       <c r="G4" s="19">
         <v>179.64000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>43522</v>
       </c>
@@ -1246,8 +1289,12 @@
       <c r="G5" s="19">
         <v>539.7299999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>43539</v>
       </c>
@@ -1269,8 +1316,12 @@
       <c r="G6" s="19">
         <v>167.44</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>43556</v>
       </c>
@@ -1292,8 +1343,12 @@
       <c r="G7" s="19">
         <v>299.40000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>43573</v>
       </c>
@@ -1315,8 +1370,12 @@
       <c r="G8" s="19">
         <v>149.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>43590</v>
       </c>
@@ -1338,8 +1397,12 @@
       <c r="G9" s="19">
         <v>449.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>43607</v>
       </c>
@@ -1361,8 +1424,12 @@
       <c r="G10" s="19">
         <v>63.68</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>43624</v>
       </c>
@@ -1384,8 +1451,12 @@
       <c r="G11" s="19">
         <v>539.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>43641</v>
       </c>
@@ -1407,8 +1478,12 @@
       <c r="G12" s="19">
         <v>449.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>43658</v>
       </c>
@@ -1430,8 +1505,12 @@
       <c r="G13" s="19">
         <v>57.71</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>43675</v>
       </c>
@@ -1453,8 +1532,12 @@
       <c r="G14" s="19">
         <v>1619.1899999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>43692</v>
       </c>
@@ -1476,8 +1559,12 @@
       <c r="G15" s="19">
         <v>174.65</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>43709</v>
       </c>
@@ -1499,8 +1586,12 @@
       <c r="G16" s="19">
         <v>250</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>43726</v>
       </c>
@@ -1522,8 +1613,12 @@
       <c r="G17" s="19">
         <v>255.84</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>43743</v>
       </c>
@@ -1545,8 +1640,12 @@
       <c r="G18" s="19">
         <v>251.72</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>43760</v>
       </c>
@@ -1568,8 +1667,12 @@
       <c r="G19" s="19">
         <v>575.36</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>43777</v>
       </c>
@@ -1591,8 +1694,12 @@
       <c r="G20" s="19">
         <v>299.84999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>43794</v>
       </c>
@@ -1614,8 +1721,12 @@
       <c r="G21" s="19">
         <v>479.04</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>43811</v>
       </c>
@@ -1637,8 +1748,12 @@
       <c r="G22" s="19">
         <v>86.43</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>43828</v>
       </c>
@@ -1660,8 +1775,12 @@
       <c r="G23" s="19">
         <v>1183.26</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>43845</v>
       </c>
@@ -1683,8 +1802,12 @@
       <c r="G24" s="19">
         <v>413.54</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>43862</v>
       </c>
@@ -1706,8 +1829,12 @@
       <c r="G25" s="19">
         <v>1305</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>43879</v>
       </c>
@@ -1729,8 +1856,12 @@
       <c r="G26" s="19">
         <v>19.96</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>43897</v>
       </c>
@@ -1752,8 +1883,12 @@
       <c r="G27" s="19">
         <v>139.92999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>43914</v>
       </c>
@@ -1775,8 +1910,12 @@
       <c r="G28" s="19">
         <v>249.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>43931</v>
       </c>
@@ -1798,8 +1937,12 @@
       <c r="G29" s="19">
         <v>131.34</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>43948</v>
       </c>
@@ -1821,8 +1964,12 @@
       <c r="G30" s="19">
         <v>479.04</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>43965</v>
       </c>
@@ -1844,8 +1991,12 @@
       <c r="G31" s="19">
         <v>68.37</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>43982</v>
       </c>
@@ -1867,8 +2018,12 @@
       <c r="G32" s="19">
         <v>719.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>43999</v>
       </c>
@@ -1890,8 +2045,12 @@
       <c r="G33" s="19">
         <v>625</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>44016</v>
       </c>
@@ -1913,8 +2072,12 @@
       <c r="G34" s="19">
         <v>309.38</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>44033</v>
       </c>
@@ -1936,8 +2099,12 @@
       <c r="G35" s="19">
         <v>686.95</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>44050</v>
       </c>
@@ -1959,8 +2126,12 @@
       <c r="G36" s="19">
         <v>1005.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>44067</v>
       </c>
@@ -1982,8 +2153,12 @@
       <c r="G37" s="19">
         <v>825</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>44084</v>
       </c>
@@ -2005,8 +2180,12 @@
       <c r="G38" s="19">
         <v>9.0300000000000011</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>44101</v>
       </c>
@@ -2028,8 +2207,12 @@
       <c r="G39" s="19">
         <v>151.24</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>44118</v>
       </c>
@@ -2051,8 +2234,12 @@
       <c r="G40" s="19">
         <v>1139.4299999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>44135</v>
       </c>
@@ -2074,8 +2261,12 @@
       <c r="G41" s="19">
         <v>18.060000000000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>44152</v>
       </c>
@@ -2097,8 +2288,12 @@
       <c r="G42" s="19">
         <v>54.89</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>44169</v>
       </c>
@@ -2120,8 +2315,12 @@
       <c r="G43" s="19">
         <v>1879.06</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>44186</v>
       </c>
@@ -2142,6 +2341,10 @@
       </c>
       <c r="G44" s="19">
         <v>139.72</v>
+      </c>
+      <c r="H44" s="6" t="b">
+        <f>Table1[[#This Row],[Units]]&lt;10</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>